<commit_message>
fix excel cell autosize
</commit_message>
<xml_diff>
--- a/maps/tilemaps/Braunschweig_SQ.xlsx
+++ b/maps/tilemaps/Braunschweig_SQ.xlsx
@@ -19,10 +19,10 @@
     <t>G</t>
   </si>
   <si>
-    <t>B</t>
+    <t>W</t>
   </si>
   <si>
-    <t>W</t>
+    <t>B</t>
   </si>
 </sst>
 </file>
@@ -426,16 +426,16 @@
         <v>0</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>0</v>
@@ -444,7 +444,7 @@
         <v>0</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>0</v>
@@ -470,22 +470,22 @@
         <v>2</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>0</v>
@@ -514,31 +514,31 @@
         <v>2</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:14" s="1" customFormat="1" ht="45.75" customHeight="1">
@@ -552,37 +552,37 @@
         <v>0</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M4" s="1" t="s">
         <v>0</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:14" s="1" customFormat="1" ht="45.75" customHeight="1">
@@ -596,69 +596,69 @@
         <v>1</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>1</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:14" s="1" customFormat="1" ht="45.75" customHeight="1">
       <c r="A6" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>0</v>
@@ -667,10 +667,10 @@
         <v>0</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:14" s="1" customFormat="1" ht="45.75" customHeight="1">
@@ -678,25 +678,25 @@
         <v>0</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>1</v>
@@ -705,10 +705,10 @@
         <v>2</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M7" s="1" t="s">
         <v>2</v>
@@ -719,40 +719,40 @@
     </row>
     <row r="8" spans="1:14" s="1" customFormat="1" ht="45.75" customHeight="1">
       <c r="A8" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K8" s="1" t="s">
         <v>2</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M8" s="1" t="s">
         <v>2</v>
@@ -763,46 +763,46 @@
     </row>
     <row r="9" spans="1:14" s="1" customFormat="1" ht="45.75" customHeight="1">
       <c r="A9" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>2</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L9" s="1" t="s">
         <v>2</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:14" s="1" customFormat="1" ht="45.75" customHeight="1">
@@ -810,40 +810,40 @@
         <v>0</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>1</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K10" s="1" t="s">
         <v>1</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N10" s="1" t="s">
         <v>0</v>
@@ -854,13 +854,13 @@
         <v>0</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>2</v>
@@ -869,25 +869,25 @@
         <v>0</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>1</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>2</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N11" s="1" t="s">
         <v>0</v>
@@ -895,37 +895,37 @@
     </row>
     <row r="12" spans="1:14" s="1" customFormat="1" ht="45.75" customHeight="1">
       <c r="A12" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>0</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>1</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L12" s="1" t="s">
         <v>0</v>
@@ -934,7 +934,7 @@
         <v>0</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:14" s="1" customFormat="1" ht="45.75" customHeight="1">
@@ -945,16 +945,16 @@
         <v>0</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>1</v>
@@ -963,13 +963,13 @@
         <v>1</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L13" s="1" t="s">
         <v>0</v>
@@ -989,16 +989,16 @@
         <v>0</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>1</v>
@@ -1007,7 +1007,7 @@
         <v>0</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J14" s="1" t="s">
         <v>0</v>
@@ -1016,7 +1016,7 @@
         <v>0</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M14" s="1" t="s">
         <v>0</v>

</xml_diff>